<commit_message>
Updated the issues #12 and #16
</commit_message>
<xml_diff>
--- a/Costestimate.xlsx
+++ b/Costestimate.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538308\Documents\gdp\GDP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538098\Documents\563\GDP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360923C4-EF1F-4824-8C0C-FA566F40C686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,9 +49,6 @@
     <t>UI Developer</t>
   </si>
   <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
     <t>QA Analyst</t>
   </si>
   <si>
@@ -141,12 +137,15 @@
   </si>
   <si>
     <t>Vishal Reddy Vennavaram</t>
+  </si>
+  <si>
+    <t>Backend  Developer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -651,26 +650,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -683,50 +682,50 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8">
         <v>340</v>
@@ -744,10 +743,10 @@
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="10">
         <v>70</v>
@@ -755,9 +754,9 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="8">
         <v>340</v>
@@ -775,10 +774,10 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I12" s="10">
         <v>45</v>
@@ -786,9 +785,9 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8">
         <v>340</v>
@@ -817,9 +816,9 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <f>--D8</f>
@@ -836,7 +835,7 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>4</v>
@@ -847,9 +846,9 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -865,10 +864,10 @@
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I15" s="10">
         <v>55</v>
@@ -876,9 +875,9 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -894,10 +893,10 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="I16" s="10">
         <v>58</v>
@@ -905,9 +904,9 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -925,9 +924,9 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8">
         <v>340</v>
@@ -949,9 +948,9 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -974,9 +973,9 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -999,9 +998,9 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -1024,9 +1023,9 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8">
         <v>340</v>
@@ -1049,9 +1048,9 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="8">
         <v>340</v>
@@ -1068,7 +1067,7 @@
         <v>20400</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>